<commit_message>
WAY Corrector - تحديث الملف: 24/11/2025, 00:21:27
</commit_message>
<xml_diff>
--- a/password.xlsx
+++ b/password.xlsx
@@ -407,7 +407,7 @@
         <v>!!&lt;Z&amp;n)2nq9Z</v>
       </c>
       <c r="B1" t="str">
-        <v>used</v>
+        <v>https://mcq-app.github.io/WAY/MCQ0.xlsx</v>
       </c>
     </row>
     <row r="2">
@@ -415,7 +415,7 @@
         <v>!!=JLRP&amp;1feWD=vh</v>
       </c>
       <c r="B2" t="str">
-        <v/>
+        <v>https://mcq-app.github.io/WAY/MCQ1.xlsx</v>
       </c>
     </row>
     <row r="3">

</xml_diff>